<commit_message>
delfault hero icon and rank fix
</commit_message>
<xml_diff>
--- a/Design/config/ForceConfig.xlsx
+++ b/Design/config/ForceConfig.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>序列</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -167,6 +167,14 @@
   </si>
   <si>
     <t>#A385AD</t>
+  </si>
+  <si>
+    <t>#CCCCCC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在野</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -563,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -799,6 +807,20 @@
       </c>
       <c r="D16" s="5" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>99</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="4">
+        <v>100020</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>